<commit_message>
Refactor database schema migration
Optimize image compression algorithm.
</commit_message>
<xml_diff>
--- a/sensorCSV/SAG1_sensor_data_with_decimal_filtered_updated02.xlsx
+++ b/sensorCSV/SAG1_sensor_data_with_decimal_filtered_updated02.xlsx
@@ -3834,7 +3834,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45725.28379443287</v>
+        <v>45725.2840490625</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45725.28381615741</v>
+        <v>45725.28407078703</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -3908,7 +3908,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45725.28383988426</v>
+        <v>45725.28409451389</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -3945,7 +3945,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45725.78393704861</v>
+        <v>45725.78419167824</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -3982,7 +3982,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45725.78395944444</v>
+        <v>45725.78421407408</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -4019,7 +4019,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45725.78398240741</v>
+        <v>45725.78423703703</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -4056,7 +4056,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45726.2840793287</v>
+        <v>45726.28433395833</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -4093,7 +4093,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45726.28410148148</v>
+        <v>45726.28435611111</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -4130,7 +4130,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45726.28412525463</v>
+        <v>45726.28437988426</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -4167,7 +4167,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45726.78422107639</v>
+        <v>45726.78447570602</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -4204,7 +4204,7 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45726.7842433912</v>
+        <v>45726.78449802083</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45726.78426665509</v>
+        <v>45726.78452128472</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -4278,7 +4278,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45727.28436325231</v>
+        <v>45727.28461788195</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -4315,7 +4315,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45727.28438563657</v>
+        <v>45727.2846402662</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -4352,7 +4352,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45727.28440849537</v>
+        <v>45727.284663125</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -4389,7 +4389,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45727.78450625</v>
+        <v>45727.78476087963</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -4426,7 +4426,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45727.78452762731</v>
+        <v>45727.78478225695</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45727.78455077546</v>
+        <v>45727.78480540509</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -4500,7 +4500,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45728.28464791667</v>
+        <v>45728.28490254629</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45728.28466966435</v>
+        <v>45728.28492429398</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -4574,7 +4574,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45728.2846928125</v>
+        <v>45728.28494744213</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45728.32236603009</v>
+        <v>45728.32262065972</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -4648,7 +4648,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45728.32238929398</v>
+        <v>45728.32264392361</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -4685,7 +4685,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45728.32241254629</v>
+        <v>45728.32266717593</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -4722,7 +4722,7 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45728.82251016203</v>
+        <v>45728.82276479166</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -4759,7 +4759,7 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45728.8225322338</v>
+        <v>45728.82278686343</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -4796,7 +4796,7 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45728.82255538194</v>
+        <v>45728.82281001157</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -4833,7 +4833,7 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45729.32265225695</v>
+        <v>45729.32290688658</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45729.32267420139</v>
+        <v>45729.32292883102</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -4907,7 +4907,7 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45729.32269775463</v>
+        <v>45729.32295238426</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>

</xml_diff>